<commit_message>
attempt to get trilateration working
</commit_message>
<xml_diff>
--- a/Datasets_Network.xlsx
+++ b/Datasets_Network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212581239\Documents\Edison\MSU\824\Project\BluetoothCSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\Desktop\bluetoothcis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E67D33C-CAA2-41AF-BD4F-44F6BFA7F8B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A54F5E-8DFD-46FC-A07F-D71FCD608F30}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="465" windowWidth="24765" windowHeight="15000" activeTab="2" xr2:uid="{FE5497F7-7CD0-894E-AF87-E3AD65B3B9C0}"/>
+    <workbookView xWindow="735" yWindow="465" windowWidth="24765" windowHeight="15000" activeTab="5" xr2:uid="{FE5497F7-7CD0-894E-AF87-E3AD65B3B9C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="12" r:id="rId1"/>
@@ -35,6 +35,12 @@
     <sheet name="BLE3_6FT" sheetId="13" r:id="rId20"/>
     <sheet name="BLE3_8FT" sheetId="16" r:id="rId21"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'EX1'!$E$1:$E$210</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'EX2'!$E$1:$E$202</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'EX3'!$E$1:$E$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'EX4'!$E$1:$E$210</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13394" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13334" uniqueCount="50">
   <si>
     <t xml:space="preserve">BLE1 </t>
   </si>
@@ -176,7 +182,28 @@
     <t>Y and X coordinates</t>
   </si>
   <si>
-    <t>2 </t>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Node1</t>
+  </si>
+  <si>
+    <t>Node2</t>
+  </si>
+  <si>
+    <t>Node3</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>67,0</t>
+  </si>
+  <si>
+    <t>0,52</t>
+  </si>
+  <si>
+    <t>cm</t>
   </si>
 </sst>
 </file>
@@ -184,7 +211,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -230,7 +257,7 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17549,9 +17576,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EFCB27-EE60-A546-A8ED-7261AFA041F0}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17559,44 +17588,68 @@
     <col min="2" max="2" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -17604,7 +17657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -17612,7 +17665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -17620,7 +17673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -21025,10 +21078,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B48255-141B-AE42-97CD-E635C4D7380F}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -21092,7 +21146,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43432</v>
       </c>
@@ -21148,7 +21202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43432</v>
       </c>
@@ -21260,7 +21314,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43432</v>
       </c>
@@ -21316,7 +21370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43432</v>
       </c>
@@ -21428,7 +21482,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43432</v>
       </c>
@@ -21484,7 +21538,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>43432</v>
       </c>
@@ -21596,7 +21650,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43432</v>
       </c>
@@ -21652,7 +21706,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43432</v>
       </c>
@@ -21764,7 +21818,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43432</v>
       </c>
@@ -21820,7 +21874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>43432</v>
       </c>
@@ -21932,7 +21986,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43432</v>
       </c>
@@ -21988,7 +22042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43432</v>
       </c>
@@ -22100,7 +22154,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43432</v>
       </c>
@@ -22156,7 +22210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43432</v>
       </c>
@@ -22268,7 +22322,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>43432</v>
       </c>
@@ -22324,7 +22378,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>43432</v>
       </c>
@@ -22436,7 +22490,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43432</v>
       </c>
@@ -22492,7 +22546,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>43432</v>
       </c>
@@ -22604,7 +22658,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>43432</v>
       </c>
@@ -22660,7 +22714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>43432</v>
       </c>
@@ -22772,7 +22826,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43432</v>
       </c>
@@ -22828,7 +22882,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>43432</v>
       </c>
@@ -22940,7 +22994,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>43432</v>
       </c>
@@ -22996,7 +23050,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>43432</v>
       </c>
@@ -23108,7 +23162,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43432</v>
       </c>
@@ -23164,7 +23218,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>43432</v>
       </c>
@@ -23276,7 +23330,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>43432</v>
       </c>
@@ -23332,7 +23386,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>43432</v>
       </c>
@@ -23444,7 +23498,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43432</v>
       </c>
@@ -23500,7 +23554,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43432</v>
       </c>
@@ -23612,7 +23666,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>43432</v>
       </c>
@@ -23668,7 +23722,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43432</v>
       </c>
@@ -23780,7 +23834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>43432</v>
       </c>
@@ -23836,7 +23890,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>43432</v>
       </c>
@@ -23948,7 +24002,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>43432</v>
       </c>
@@ -24004,7 +24058,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>43432</v>
       </c>
@@ -24116,7 +24170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>43432</v>
       </c>
@@ -24172,7 +24226,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>43432</v>
       </c>
@@ -24284,7 +24338,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>43432</v>
       </c>
@@ -24340,7 +24394,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>43432</v>
       </c>
@@ -24452,7 +24506,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>43432</v>
       </c>
@@ -24508,7 +24562,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>43432</v>
       </c>
@@ -24620,7 +24674,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>43432</v>
       </c>
@@ -24676,7 +24730,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>43432</v>
       </c>
@@ -24788,7 +24842,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>43432</v>
       </c>
@@ -24844,7 +24898,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>43432</v>
       </c>
@@ -24956,7 +25010,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>43432</v>
       </c>
@@ -25012,7 +25066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>43432</v>
       </c>
@@ -25124,7 +25178,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>43432</v>
       </c>
@@ -25180,7 +25234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>43432</v>
       </c>
@@ -25292,7 +25346,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>43432</v>
       </c>
@@ -25348,7 +25402,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>43432</v>
       </c>
@@ -25460,7 +25514,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>43432</v>
       </c>
@@ -25516,7 +25570,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>43432</v>
       </c>
@@ -25628,7 +25682,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>43432</v>
       </c>
@@ -25684,7 +25738,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>43432</v>
       </c>
@@ -25796,7 +25850,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>43432</v>
       </c>
@@ -25852,7 +25906,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>43432</v>
       </c>
@@ -25964,7 +26018,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>43432</v>
       </c>
@@ -26020,7 +26074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>43432</v>
       </c>
@@ -26132,7 +26186,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>43432</v>
       </c>
@@ -26188,7 +26242,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>43432</v>
       </c>
@@ -26300,7 +26354,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>43432</v>
       </c>
@@ -26356,7 +26410,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>43432</v>
       </c>
@@ -26468,7 +26522,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>43432</v>
       </c>
@@ -26524,7 +26578,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>43432</v>
       </c>
@@ -26636,7 +26690,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>43432</v>
       </c>
@@ -26692,7 +26746,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>43432</v>
       </c>
@@ -26804,7 +26858,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>43432</v>
       </c>
@@ -26860,7 +26914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>43432</v>
       </c>
@@ -26972,7 +27026,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>43432</v>
       </c>
@@ -27028,7 +27082,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>43432</v>
       </c>
@@ -27140,7 +27194,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>43432</v>
       </c>
@@ -27196,7 +27250,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>43432</v>
       </c>
@@ -27308,7 +27362,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>43432</v>
       </c>
@@ -27364,7 +27418,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>43432</v>
       </c>
@@ -27476,7 +27530,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>43432</v>
       </c>
@@ -27532,7 +27586,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>43432</v>
       </c>
@@ -27644,7 +27698,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>43432</v>
       </c>
@@ -27700,7 +27754,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>43432</v>
       </c>
@@ -27812,7 +27866,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>43432</v>
       </c>
@@ -27868,7 +27922,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>43432</v>
       </c>
@@ -27980,7 +28034,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>43432</v>
       </c>
@@ -28036,7 +28090,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>43432</v>
       </c>
@@ -28148,7 +28202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>43432</v>
       </c>
@@ -28204,7 +28258,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>43432</v>
       </c>
@@ -28316,7 +28370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>43432</v>
       </c>
@@ -28372,7 +28426,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>43432</v>
       </c>
@@ -28484,7 +28538,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>43432</v>
       </c>
@@ -28540,7 +28594,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>43432</v>
       </c>
@@ -28652,7 +28706,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>43432</v>
       </c>
@@ -28708,7 +28762,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>43432</v>
       </c>
@@ -28820,7 +28874,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>43432</v>
       </c>
@@ -28876,7 +28930,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>43432</v>
       </c>
@@ -28988,7 +29042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>43432</v>
       </c>
@@ -29044,7 +29098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>43432</v>
       </c>
@@ -29156,7 +29210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>43432</v>
       </c>
@@ -29212,7 +29266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>43432</v>
       </c>
@@ -29324,7 +29378,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>43432</v>
       </c>
@@ -29380,7 +29434,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>43432</v>
       </c>
@@ -29492,7 +29546,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>43432</v>
       </c>
@@ -29548,7 +29602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>43432</v>
       </c>
@@ -29660,7 +29714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>43432</v>
       </c>
@@ -29716,7 +29770,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>43432</v>
       </c>
@@ -29828,7 +29882,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>43432</v>
       </c>
@@ -29884,7 +29938,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>43432</v>
       </c>
@@ -29996,7 +30050,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>43432</v>
       </c>
@@ -30052,7 +30106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>43432</v>
       </c>
@@ -30164,7 +30218,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>43432</v>
       </c>
@@ -30220,7 +30274,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>43432</v>
       </c>
@@ -30332,7 +30386,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>43432</v>
       </c>
@@ -30388,7 +30442,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>43432</v>
       </c>
@@ -30500,7 +30554,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>43432</v>
       </c>
@@ -30556,7 +30610,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>43432</v>
       </c>
@@ -30668,7 +30722,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>43432</v>
       </c>
@@ -30724,7 +30778,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>43432</v>
       </c>
@@ -30836,7 +30890,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>43432</v>
       </c>
@@ -30892,7 +30946,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>43432</v>
       </c>
@@ -31004,7 +31058,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>43432</v>
       </c>
@@ -31060,7 +31114,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>43432</v>
       </c>
@@ -31172,7 +31226,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>43432</v>
       </c>
@@ -31228,7 +31282,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>43432</v>
       </c>
@@ -31340,7 +31394,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>43432</v>
       </c>
@@ -31396,7 +31450,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>43432</v>
       </c>
@@ -31508,7 +31562,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>43432</v>
       </c>
@@ -31564,7 +31618,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>43432</v>
       </c>
@@ -31676,7 +31730,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>43432</v>
       </c>
@@ -31732,7 +31786,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>43432</v>
       </c>
@@ -31844,7 +31898,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>43432</v>
       </c>
@@ -31900,7 +31954,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>43432</v>
       </c>
@@ -32012,7 +32066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>43432</v>
       </c>
@@ -32068,7 +32122,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>43432</v>
       </c>
@@ -32180,7 +32234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>43432</v>
       </c>
@@ -32236,7 +32290,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>43432</v>
       </c>
@@ -32348,7 +32402,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>43432</v>
       </c>
@@ -32404,7 +32458,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>43432</v>
       </c>
@@ -32516,7 +32570,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>43432</v>
       </c>
@@ -32572,7 +32626,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>43432</v>
       </c>
@@ -32684,7 +32738,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>43432</v>
       </c>
@@ -32740,7 +32794,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>43432</v>
       </c>
@@ -32797,16 +32851,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E210" xr:uid="{888BBD1D-617F-48FC-8678-2AF3B73F6D7D}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F396C48A-20BD-DC4D-9493-779EDCBD6DEF}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H108" sqref="H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -32867,7 +32929,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43432</v>
       </c>
@@ -32979,7 +33041,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43432</v>
       </c>
@@ -33035,7 +33097,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43432</v>
       </c>
@@ -33147,7 +33209,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43432</v>
       </c>
@@ -33203,7 +33265,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43432</v>
       </c>
@@ -33315,7 +33377,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>43432</v>
       </c>
@@ -33371,7 +33433,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43432</v>
       </c>
@@ -33483,7 +33545,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43432</v>
       </c>
@@ -33539,7 +33601,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43432</v>
       </c>
@@ -33651,7 +33713,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>43432</v>
       </c>
@@ -33707,7 +33769,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43432</v>
       </c>
@@ -33819,7 +33881,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>43432</v>
       </c>
@@ -33875,7 +33937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43432</v>
       </c>
@@ -33987,7 +34049,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>43432</v>
       </c>
@@ -34043,7 +34105,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>43432</v>
       </c>
@@ -34155,7 +34217,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>43432</v>
       </c>
@@ -34211,7 +34273,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43432</v>
       </c>
@@ -34323,7 +34385,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>43432</v>
       </c>
@@ -34379,7 +34441,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>43432</v>
       </c>
@@ -34491,7 +34553,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>43432</v>
       </c>
@@ -34547,7 +34609,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43432</v>
       </c>
@@ -34659,7 +34721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>43432</v>
       </c>
@@ -34715,7 +34777,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>43432</v>
       </c>
@@ -34827,7 +34889,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>43432</v>
       </c>
@@ -34883,7 +34945,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43432</v>
       </c>
@@ -34995,7 +35057,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>43432</v>
       </c>
@@ -35051,7 +35113,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>43432</v>
       </c>
@@ -35163,7 +35225,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>43432</v>
       </c>
@@ -35219,7 +35281,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43432</v>
       </c>
@@ -35331,7 +35393,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43432</v>
       </c>
@@ -35387,7 +35449,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>43432</v>
       </c>
@@ -35499,7 +35561,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>43432</v>
       </c>
@@ -35555,7 +35617,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>43432</v>
       </c>
@@ -35667,7 +35729,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>43432</v>
       </c>
@@ -35723,7 +35785,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>43432</v>
       </c>
@@ -35835,7 +35897,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>43432</v>
       </c>
@@ -35891,7 +35953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>43432</v>
       </c>
@@ -36003,7 +36065,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>43432</v>
       </c>
@@ -36059,7 +36121,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>43432</v>
       </c>
@@ -36171,7 +36233,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>43432</v>
       </c>
@@ -36227,7 +36289,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>43432</v>
       </c>
@@ -36339,7 +36401,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>43432</v>
       </c>
@@ -36395,7 +36457,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>43432</v>
       </c>
@@ -36507,7 +36569,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>43432</v>
       </c>
@@ -36563,7 +36625,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>43432</v>
       </c>
@@ -36675,7 +36737,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>43432</v>
       </c>
@@ -36731,7 +36793,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>43432</v>
       </c>
@@ -36843,7 +36905,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>43432</v>
       </c>
@@ -36899,7 +36961,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>43432</v>
       </c>
@@ -37011,7 +37073,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>43432</v>
       </c>
@@ -37067,7 +37129,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>43432</v>
       </c>
@@ -37179,7 +37241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>43432</v>
       </c>
@@ -37235,7 +37297,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>43432</v>
       </c>
@@ -37347,7 +37409,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>43432</v>
       </c>
@@ -37403,7 +37465,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>43432</v>
       </c>
@@ -37515,7 +37577,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>43432</v>
       </c>
@@ -37571,7 +37633,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>43432</v>
       </c>
@@ -37683,7 +37745,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>43432</v>
       </c>
@@ -37739,7 +37801,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>43432</v>
       </c>
@@ -37851,7 +37913,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>43432</v>
       </c>
@@ -37907,7 +37969,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>43432</v>
       </c>
@@ -38019,7 +38081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>43432</v>
       </c>
@@ -38075,7 +38137,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>43432</v>
       </c>
@@ -38187,7 +38249,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>43432</v>
       </c>
@@ -38243,7 +38305,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>43432</v>
       </c>
@@ -38355,7 +38417,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>43432</v>
       </c>
@@ -38411,7 +38473,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>43432</v>
       </c>
@@ -38523,7 +38585,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>43432</v>
       </c>
@@ -38579,7 +38641,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>43432</v>
       </c>
@@ -38691,7 +38753,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>43432</v>
       </c>
@@ -38747,7 +38809,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>43432</v>
       </c>
@@ -38859,7 +38921,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>43432</v>
       </c>
@@ -38915,7 +38977,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>43432</v>
       </c>
@@ -39027,7 +39089,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>43432</v>
       </c>
@@ -39083,7 +39145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>43432</v>
       </c>
@@ -39195,7 +39257,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>43432</v>
       </c>
@@ -39251,7 +39313,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>43432</v>
       </c>
@@ -39363,7 +39425,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>43432</v>
       </c>
@@ -39419,7 +39481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>43432</v>
       </c>
@@ -39531,7 +39593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>43432</v>
       </c>
@@ -39587,7 +39649,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>43432</v>
       </c>
@@ -39699,7 +39761,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>43432</v>
       </c>
@@ -39755,7 +39817,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>43432</v>
       </c>
@@ -39867,7 +39929,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>43432</v>
       </c>
@@ -39923,7 +39985,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>43432</v>
       </c>
@@ -40035,7 +40097,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>43432</v>
       </c>
@@ -40091,7 +40153,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>43432</v>
       </c>
@@ -40203,7 +40265,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>43432</v>
       </c>
@@ -40259,7 +40321,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>43432</v>
       </c>
@@ -40371,7 +40433,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>43432</v>
       </c>
@@ -40427,7 +40489,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>43432</v>
       </c>
@@ -40539,7 +40601,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>43432</v>
       </c>
@@ -40595,7 +40657,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>43432</v>
       </c>
@@ -40707,7 +40769,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>43432</v>
       </c>
@@ -40763,7 +40825,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>43432</v>
       </c>
@@ -40875,7 +40937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>43432</v>
       </c>
@@ -40931,7 +40993,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>43432</v>
       </c>
@@ -41043,7 +41105,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>43432</v>
       </c>
@@ -41099,7 +41161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>43432</v>
       </c>
@@ -41211,7 +41273,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>43432</v>
       </c>
@@ -41267,7 +41329,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>43432</v>
       </c>
@@ -41379,7 +41441,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>43432</v>
       </c>
@@ -41435,7 +41497,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>43432</v>
       </c>
@@ -41547,7 +41609,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>43432</v>
       </c>
@@ -41603,7 +41665,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>43432</v>
       </c>
@@ -41715,7 +41777,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>43432</v>
       </c>
@@ -41771,7 +41833,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>43432</v>
       </c>
@@ -41883,7 +41945,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>43432</v>
       </c>
@@ -41939,7 +42001,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>43432</v>
       </c>
@@ -42051,7 +42113,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>43432</v>
       </c>
@@ -42107,7 +42169,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>43432</v>
       </c>
@@ -42219,7 +42281,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>43432</v>
       </c>
@@ -42275,7 +42337,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>43432</v>
       </c>
@@ -42387,7 +42449,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>43432</v>
       </c>
@@ -42443,7 +42505,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>43432</v>
       </c>
@@ -42555,7 +42617,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>43432</v>
       </c>
@@ -42611,7 +42673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>43432</v>
       </c>
@@ -42723,7 +42785,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>43432</v>
       </c>
@@ -42779,7 +42841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>43432</v>
       </c>
@@ -42891,7 +42953,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>43432</v>
       </c>
@@ -42947,7 +43009,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>43432</v>
       </c>
@@ -43059,7 +43121,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>43432</v>
       </c>
@@ -43115,7 +43177,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>43432</v>
       </c>
@@ -43227,7 +43289,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>43432</v>
       </c>
@@ -43283,7 +43345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>43432</v>
       </c>
@@ -43395,7 +43457,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>43432</v>
       </c>
@@ -43451,7 +43513,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>43432</v>
       </c>
@@ -43563,7 +43625,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>43432</v>
       </c>
@@ -43675,7 +43737,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>43432</v>
       </c>
@@ -43787,7 +43849,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>43432</v>
       </c>
@@ -43899,7 +43961,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>43432</v>
       </c>
@@ -44011,7 +44073,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>43432</v>
       </c>
@@ -44124,16 +44186,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E202" xr:uid="{DC604E12-35F9-4C41-A63D-122B4AA2CEF7}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5975EB95-B45C-8A4F-A0A8-070BBDC42FB6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R213"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -44194,7 +44264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43432</v>
       </c>
@@ -44250,7 +44320,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43432</v>
       </c>
@@ -44362,7 +44432,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43432</v>
       </c>
@@ -44418,7 +44488,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43432</v>
       </c>
@@ -44530,7 +44600,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43432</v>
       </c>
@@ -44586,7 +44656,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>43432</v>
       </c>
@@ -44698,7 +44768,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43432</v>
       </c>
@@ -44754,7 +44824,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43432</v>
       </c>
@@ -44866,7 +44936,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43432</v>
       </c>
@@ -44922,7 +44992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>43432</v>
       </c>
@@ -45034,7 +45104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43432</v>
       </c>
@@ -45090,7 +45160,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43432</v>
       </c>
@@ -45202,7 +45272,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43432</v>
       </c>
@@ -45258,7 +45328,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43432</v>
       </c>
@@ -45370,7 +45440,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>43432</v>
       </c>
@@ -45426,7 +45496,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>43432</v>
       </c>
@@ -45538,7 +45608,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43432</v>
       </c>
@@ -45594,7 +45664,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>43432</v>
       </c>
@@ -45706,7 +45776,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>43432</v>
       </c>
@@ -45762,7 +45832,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>43432</v>
       </c>
@@ -45874,7 +45944,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43432</v>
       </c>
@@ -45930,7 +46000,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>43432</v>
       </c>
@@ -46042,7 +46112,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>43432</v>
       </c>
@@ -46098,7 +46168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>43432</v>
       </c>
@@ -46210,7 +46280,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43432</v>
       </c>
@@ -46266,7 +46336,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>43432</v>
       </c>
@@ -46378,7 +46448,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>43432</v>
       </c>
@@ -46434,7 +46504,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>43432</v>
       </c>
@@ -46546,7 +46616,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43432</v>
       </c>
@@ -46602,7 +46672,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43432</v>
       </c>
@@ -46714,7 +46784,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>43432</v>
       </c>
@@ -46770,7 +46840,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43432</v>
       </c>
@@ -46882,7 +46952,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>43432</v>
       </c>
@@ -46938,7 +47008,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>43432</v>
       </c>
@@ -47050,7 +47120,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>43432</v>
       </c>
@@ -47106,7 +47176,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>43432</v>
       </c>
@@ -47218,7 +47288,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>43432</v>
       </c>
@@ -47274,7 +47344,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>43432</v>
       </c>
@@ -47386,7 +47456,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>43432</v>
       </c>
@@ -47442,7 +47512,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>43432</v>
       </c>
@@ -47554,7 +47624,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>43432</v>
       </c>
@@ -47610,7 +47680,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>43432</v>
       </c>
@@ -47722,7 +47792,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>43432</v>
       </c>
@@ -47778,7 +47848,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>43432</v>
       </c>
@@ -47890,7 +47960,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>43432</v>
       </c>
@@ -47946,7 +48016,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>43432</v>
       </c>
@@ -48058,7 +48128,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>43432</v>
       </c>
@@ -48114,7 +48184,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>43432</v>
       </c>
@@ -48226,7 +48296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>43432</v>
       </c>
@@ -48282,7 +48352,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>43432</v>
       </c>
@@ -48394,7 +48464,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>43432</v>
       </c>
@@ -48450,7 +48520,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>43432</v>
       </c>
@@ -48562,7 +48632,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>43432</v>
       </c>
@@ -48618,7 +48688,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>43432</v>
       </c>
@@ -48730,7 +48800,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>43432</v>
       </c>
@@ -48786,7 +48856,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>43432</v>
       </c>
@@ -48898,7 +48968,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>43432</v>
       </c>
@@ -48954,7 +49024,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>43432</v>
       </c>
@@ -49066,7 +49136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>43432</v>
       </c>
@@ -49122,7 +49192,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>43432</v>
       </c>
@@ -49234,7 +49304,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>43432</v>
       </c>
@@ -49290,7 +49360,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>43432</v>
       </c>
@@ -49402,7 +49472,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>43432</v>
       </c>
@@ -49458,7 +49528,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>43432</v>
       </c>
@@ -49570,7 +49640,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>43432</v>
       </c>
@@ -49626,7 +49696,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>43432</v>
       </c>
@@ -49738,7 +49808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>43432</v>
       </c>
@@ -49794,7 +49864,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>43432</v>
       </c>
@@ -49906,7 +49976,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>43432</v>
       </c>
@@ -49962,7 +50032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>43432</v>
       </c>
@@ -50074,7 +50144,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>43432</v>
       </c>
@@ -50130,7 +50200,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>43432</v>
       </c>
@@ -50242,7 +50312,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>43432</v>
       </c>
@@ -50298,7 +50368,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>43432</v>
       </c>
@@ -50410,7 +50480,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>43432</v>
       </c>
@@ -50466,7 +50536,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>43432</v>
       </c>
@@ -50578,7 +50648,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>43432</v>
       </c>
@@ -50634,7 +50704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>43432</v>
       </c>
@@ -50746,7 +50816,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>43432</v>
       </c>
@@ -50802,7 +50872,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>43432</v>
       </c>
@@ -50914,7 +50984,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>43432</v>
       </c>
@@ -50970,7 +51040,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>43432</v>
       </c>
@@ -51082,7 +51152,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>43432</v>
       </c>
@@ -51138,7 +51208,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>43432</v>
       </c>
@@ -51250,7 +51320,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>43432</v>
       </c>
@@ -51306,7 +51376,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>43432</v>
       </c>
@@ -51418,7 +51488,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>43432</v>
       </c>
@@ -51474,7 +51544,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>43432</v>
       </c>
@@ -51586,7 +51656,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>43432</v>
       </c>
@@ -51642,7 +51712,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>43432</v>
       </c>
@@ -51754,7 +51824,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>43432</v>
       </c>
@@ -51810,7 +51880,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>43432</v>
       </c>
@@ -51922,7 +51992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>43432</v>
       </c>
@@ -51978,7 +52048,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>43432</v>
       </c>
@@ -52090,7 +52160,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>43432</v>
       </c>
@@ -52146,7 +52216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>43432</v>
       </c>
@@ -52258,7 +52328,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>43432</v>
       </c>
@@ -52314,7 +52384,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>43432</v>
       </c>
@@ -52426,7 +52496,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>43432</v>
       </c>
@@ -52482,7 +52552,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>43432</v>
       </c>
@@ -52594,7 +52664,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>43432</v>
       </c>
@@ -52650,7 +52720,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>43432</v>
       </c>
@@ -52762,7 +52832,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>43432</v>
       </c>
@@ -52818,7 +52888,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>43432</v>
       </c>
@@ -52930,7 +53000,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>43432</v>
       </c>
@@ -52986,7 +53056,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>43432</v>
       </c>
@@ -53098,7 +53168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>43432</v>
       </c>
@@ -53154,7 +53224,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>43432</v>
       </c>
@@ -53266,7 +53336,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>43432</v>
       </c>
@@ -53322,7 +53392,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>43432</v>
       </c>
@@ -53434,7 +53504,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>43432</v>
       </c>
@@ -53490,7 +53560,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>43432</v>
       </c>
@@ -53602,7 +53672,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>43432</v>
       </c>
@@ -53658,7 +53728,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>43432</v>
       </c>
@@ -53770,7 +53840,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>43432</v>
       </c>
@@ -53826,7 +53896,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>43432</v>
       </c>
@@ -53938,7 +54008,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>43432</v>
       </c>
@@ -53994,7 +54064,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>43432</v>
       </c>
@@ -54106,7 +54176,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>43432</v>
       </c>
@@ -54162,7 +54232,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>43432</v>
       </c>
@@ -54274,7 +54344,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>43432</v>
       </c>
@@ -54330,7 +54400,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>43432</v>
       </c>
@@ -54442,7 +54512,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>43432</v>
       </c>
@@ -54498,7 +54568,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>43432</v>
       </c>
@@ -54610,7 +54680,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>43432</v>
       </c>
@@ -54666,7 +54736,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>43432</v>
       </c>
@@ -54778,7 +54848,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>43432</v>
       </c>
@@ -54834,7 +54904,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>43432</v>
       </c>
@@ -54946,7 +55016,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>43432</v>
       </c>
@@ -55002,7 +55072,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>43432</v>
       </c>
@@ -55114,7 +55184,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>43432</v>
       </c>
@@ -55170,7 +55240,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>43432</v>
       </c>
@@ -55282,7 +55352,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>43432</v>
       </c>
@@ -55338,7 +55408,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>43432</v>
       </c>
@@ -55450,7 +55520,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>43432</v>
       </c>
@@ -55506,7 +55576,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>43432</v>
       </c>
@@ -55618,7 +55688,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>43432</v>
       </c>
@@ -55674,7 +55744,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>43432</v>
       </c>
@@ -55786,7 +55856,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>43432</v>
       </c>
@@ -55842,7 +55912,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>43432</v>
       </c>
@@ -55954,7 +56024,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <v>43432</v>
       </c>
@@ -56010,7 +56080,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
         <v>43432</v>
       </c>
@@ -56067,6 +56137,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E213" xr:uid="{DFE4D983-05D8-415D-9750-FBE210D8B83D}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -56075,8 +56152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00673D01-E821-9F47-9E73-EC829E2F7555}">
   <dimension ref="A1:R210"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -56542,8 +56619,8 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
-        <v>42</v>
+      <c r="E9">
+        <v>2</v>
       </c>
       <c r="F9" t="s">
         <v>25</v>
@@ -56710,8 +56787,8 @@
       <c r="D12" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="s">
-        <v>42</v>
+      <c r="E12">
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>25</v>
@@ -56878,8 +56955,8 @@
       <c r="D15" t="s">
         <v>23</v>
       </c>
-      <c r="E15" t="s">
-        <v>42</v>
+      <c r="E15">
+        <v>2</v>
       </c>
       <c r="F15" t="s">
         <v>25</v>
@@ -57046,8 +57123,8 @@
       <c r="D18" t="s">
         <v>23</v>
       </c>
-      <c r="E18" t="s">
-        <v>42</v>
+      <c r="E18">
+        <v>2</v>
       </c>
       <c r="F18" t="s">
         <v>25</v>
@@ -57214,8 +57291,8 @@
       <c r="D21" t="s">
         <v>23</v>
       </c>
-      <c r="E21" t="s">
-        <v>42</v>
+      <c r="E21">
+        <v>2</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
@@ -57382,8 +57459,8 @@
       <c r="D24" t="s">
         <v>23</v>
       </c>
-      <c r="E24" t="s">
-        <v>42</v>
+      <c r="E24">
+        <v>2</v>
       </c>
       <c r="F24" t="s">
         <v>25</v>
@@ -57550,8 +57627,8 @@
       <c r="D27" t="s">
         <v>23</v>
       </c>
-      <c r="E27" t="s">
-        <v>42</v>
+      <c r="E27">
+        <v>2</v>
       </c>
       <c r="F27" t="s">
         <v>25</v>
@@ -57718,8 +57795,8 @@
       <c r="D30" t="s">
         <v>23</v>
       </c>
-      <c r="E30" t="s">
-        <v>42</v>
+      <c r="E30">
+        <v>2</v>
       </c>
       <c r="F30" t="s">
         <v>25</v>
@@ -57886,8 +57963,8 @@
       <c r="D33" t="s">
         <v>23</v>
       </c>
-      <c r="E33" t="s">
-        <v>42</v>
+      <c r="E33">
+        <v>2</v>
       </c>
       <c r="F33" t="s">
         <v>25</v>
@@ -58054,8 +58131,8 @@
       <c r="D36" t="s">
         <v>23</v>
       </c>
-      <c r="E36" t="s">
-        <v>42</v>
+      <c r="E36">
+        <v>2</v>
       </c>
       <c r="F36" t="s">
         <v>25</v>
@@ -58222,8 +58299,8 @@
       <c r="D39" t="s">
         <v>23</v>
       </c>
-      <c r="E39" t="s">
-        <v>42</v>
+      <c r="E39">
+        <v>2</v>
       </c>
       <c r="F39" t="s">
         <v>25</v>
@@ -58390,8 +58467,8 @@
       <c r="D42" t="s">
         <v>23</v>
       </c>
-      <c r="E42" t="s">
-        <v>42</v>
+      <c r="E42">
+        <v>2</v>
       </c>
       <c r="F42" t="s">
         <v>25</v>
@@ -58558,8 +58635,8 @@
       <c r="D45" t="s">
         <v>23</v>
       </c>
-      <c r="E45" t="s">
-        <v>42</v>
+      <c r="E45">
+        <v>2</v>
       </c>
       <c r="F45" t="s">
         <v>25</v>
@@ -58726,8 +58803,8 @@
       <c r="D48" t="s">
         <v>23</v>
       </c>
-      <c r="E48" t="s">
-        <v>42</v>
+      <c r="E48">
+        <v>2</v>
       </c>
       <c r="F48" t="s">
         <v>25</v>
@@ -58894,8 +58971,8 @@
       <c r="D51" t="s">
         <v>23</v>
       </c>
-      <c r="E51" t="s">
-        <v>42</v>
+      <c r="E51">
+        <v>2</v>
       </c>
       <c r="F51" t="s">
         <v>25</v>
@@ -59062,8 +59139,8 @@
       <c r="D54" t="s">
         <v>23</v>
       </c>
-      <c r="E54" t="s">
-        <v>42</v>
+      <c r="E54">
+        <v>2</v>
       </c>
       <c r="F54" t="s">
         <v>25</v>
@@ -59230,8 +59307,8 @@
       <c r="D57" t="s">
         <v>23</v>
       </c>
-      <c r="E57" t="s">
-        <v>42</v>
+      <c r="E57">
+        <v>2</v>
       </c>
       <c r="F57" t="s">
         <v>25</v>
@@ -59398,8 +59475,8 @@
       <c r="D60" t="s">
         <v>23</v>
       </c>
-      <c r="E60" t="s">
-        <v>42</v>
+      <c r="E60">
+        <v>2</v>
       </c>
       <c r="F60" t="s">
         <v>25</v>
@@ -59566,8 +59643,8 @@
       <c r="D63" t="s">
         <v>23</v>
       </c>
-      <c r="E63" t="s">
-        <v>42</v>
+      <c r="E63">
+        <v>2</v>
       </c>
       <c r="F63" t="s">
         <v>25</v>
@@ -59734,8 +59811,8 @@
       <c r="D66" t="s">
         <v>23</v>
       </c>
-      <c r="E66" t="s">
-        <v>42</v>
+      <c r="E66">
+        <v>2</v>
       </c>
       <c r="F66" t="s">
         <v>25</v>
@@ -59902,8 +59979,8 @@
       <c r="D69" t="s">
         <v>23</v>
       </c>
-      <c r="E69" t="s">
-        <v>42</v>
+      <c r="E69">
+        <v>2</v>
       </c>
       <c r="F69" t="s">
         <v>25</v>
@@ -60070,8 +60147,8 @@
       <c r="D72" t="s">
         <v>23</v>
       </c>
-      <c r="E72" t="s">
-        <v>42</v>
+      <c r="E72">
+        <v>2</v>
       </c>
       <c r="F72" t="s">
         <v>25</v>
@@ -60238,8 +60315,8 @@
       <c r="D75" t="s">
         <v>23</v>
       </c>
-      <c r="E75" t="s">
-        <v>42</v>
+      <c r="E75">
+        <v>2</v>
       </c>
       <c r="F75" t="s">
         <v>25</v>
@@ -60406,8 +60483,8 @@
       <c r="D78" t="s">
         <v>23</v>
       </c>
-      <c r="E78" t="s">
-        <v>42</v>
+      <c r="E78">
+        <v>2</v>
       </c>
       <c r="F78" t="s">
         <v>25</v>
@@ -60574,8 +60651,8 @@
       <c r="D81" t="s">
         <v>23</v>
       </c>
-      <c r="E81" t="s">
-        <v>42</v>
+      <c r="E81">
+        <v>2</v>
       </c>
       <c r="F81" t="s">
         <v>25</v>
@@ -60742,8 +60819,8 @@
       <c r="D84" t="s">
         <v>23</v>
       </c>
-      <c r="E84" t="s">
-        <v>42</v>
+      <c r="E84">
+        <v>2</v>
       </c>
       <c r="F84" t="s">
         <v>25</v>
@@ -60910,8 +60987,8 @@
       <c r="D87" t="s">
         <v>23</v>
       </c>
-      <c r="E87" t="s">
-        <v>42</v>
+      <c r="E87">
+        <v>2</v>
       </c>
       <c r="F87" t="s">
         <v>25</v>
@@ -61078,8 +61155,8 @@
       <c r="D90" t="s">
         <v>23</v>
       </c>
-      <c r="E90" t="s">
-        <v>42</v>
+      <c r="E90">
+        <v>2</v>
       </c>
       <c r="F90" t="s">
         <v>25</v>
@@ -61246,8 +61323,8 @@
       <c r="D93" t="s">
         <v>23</v>
       </c>
-      <c r="E93" t="s">
-        <v>42</v>
+      <c r="E93">
+        <v>2</v>
       </c>
       <c r="F93" t="s">
         <v>25</v>
@@ -61414,8 +61491,8 @@
       <c r="D96" t="s">
         <v>23</v>
       </c>
-      <c r="E96" t="s">
-        <v>42</v>
+      <c r="E96">
+        <v>2</v>
       </c>
       <c r="F96" t="s">
         <v>25</v>
@@ -61582,8 +61659,8 @@
       <c r="D99" t="s">
         <v>23</v>
       </c>
-      <c r="E99" t="s">
-        <v>42</v>
+      <c r="E99">
+        <v>2</v>
       </c>
       <c r="F99" t="s">
         <v>25</v>
@@ -61750,8 +61827,8 @@
       <c r="D102" t="s">
         <v>23</v>
       </c>
-      <c r="E102" t="s">
-        <v>42</v>
+      <c r="E102">
+        <v>2</v>
       </c>
       <c r="F102" t="s">
         <v>25</v>
@@ -61918,8 +61995,8 @@
       <c r="D105" t="s">
         <v>23</v>
       </c>
-      <c r="E105" t="s">
-        <v>42</v>
+      <c r="E105">
+        <v>2</v>
       </c>
       <c r="F105" t="s">
         <v>25</v>
@@ -62086,8 +62163,8 @@
       <c r="D108" t="s">
         <v>23</v>
       </c>
-      <c r="E108" t="s">
-        <v>42</v>
+      <c r="E108">
+        <v>2</v>
       </c>
       <c r="F108" t="s">
         <v>25</v>
@@ -62254,8 +62331,8 @@
       <c r="D111" t="s">
         <v>23</v>
       </c>
-      <c r="E111" t="s">
-        <v>42</v>
+      <c r="E111">
+        <v>2</v>
       </c>
       <c r="F111" t="s">
         <v>25</v>
@@ -62422,8 +62499,8 @@
       <c r="D114" t="s">
         <v>23</v>
       </c>
-      <c r="E114" t="s">
-        <v>42</v>
+      <c r="E114">
+        <v>2</v>
       </c>
       <c r="F114" t="s">
         <v>25</v>
@@ -62590,8 +62667,8 @@
       <c r="D117" t="s">
         <v>23</v>
       </c>
-      <c r="E117" t="s">
-        <v>42</v>
+      <c r="E117">
+        <v>2</v>
       </c>
       <c r="F117" t="s">
         <v>25</v>
@@ -62758,8 +62835,8 @@
       <c r="D120" t="s">
         <v>23</v>
       </c>
-      <c r="E120" t="s">
-        <v>42</v>
+      <c r="E120">
+        <v>2</v>
       </c>
       <c r="F120" t="s">
         <v>25</v>
@@ -62926,8 +63003,8 @@
       <c r="D123" t="s">
         <v>23</v>
       </c>
-      <c r="E123" t="s">
-        <v>42</v>
+      <c r="E123">
+        <v>2</v>
       </c>
       <c r="F123" t="s">
         <v>25</v>
@@ -63094,8 +63171,8 @@
       <c r="D126" t="s">
         <v>23</v>
       </c>
-      <c r="E126" t="s">
-        <v>42</v>
+      <c r="E126">
+        <v>2</v>
       </c>
       <c r="F126" t="s">
         <v>25</v>
@@ -63262,8 +63339,8 @@
       <c r="D129" t="s">
         <v>23</v>
       </c>
-      <c r="E129" t="s">
-        <v>42</v>
+      <c r="E129">
+        <v>2</v>
       </c>
       <c r="F129" t="s">
         <v>25</v>
@@ -63430,8 +63507,8 @@
       <c r="D132" t="s">
         <v>23</v>
       </c>
-      <c r="E132" t="s">
-        <v>42</v>
+      <c r="E132">
+        <v>2</v>
       </c>
       <c r="F132" t="s">
         <v>25</v>
@@ -63598,8 +63675,8 @@
       <c r="D135" t="s">
         <v>23</v>
       </c>
-      <c r="E135" t="s">
-        <v>42</v>
+      <c r="E135">
+        <v>2</v>
       </c>
       <c r="F135" t="s">
         <v>25</v>
@@ -63766,8 +63843,8 @@
       <c r="D138" t="s">
         <v>23</v>
       </c>
-      <c r="E138" t="s">
-        <v>42</v>
+      <c r="E138">
+        <v>2</v>
       </c>
       <c r="F138" t="s">
         <v>25</v>
@@ -63934,8 +64011,8 @@
       <c r="D141" t="s">
         <v>23</v>
       </c>
-      <c r="E141" t="s">
-        <v>42</v>
+      <c r="E141">
+        <v>2</v>
       </c>
       <c r="F141" t="s">
         <v>25</v>
@@ -64102,8 +64179,8 @@
       <c r="D144" t="s">
         <v>23</v>
       </c>
-      <c r="E144" t="s">
-        <v>42</v>
+      <c r="E144">
+        <v>2</v>
       </c>
       <c r="F144" t="s">
         <v>25</v>
@@ -64270,8 +64347,8 @@
       <c r="D147" t="s">
         <v>23</v>
       </c>
-      <c r="E147" t="s">
-        <v>42</v>
+      <c r="E147">
+        <v>2</v>
       </c>
       <c r="F147" t="s">
         <v>25</v>
@@ -64438,8 +64515,8 @@
       <c r="D150" t="s">
         <v>23</v>
       </c>
-      <c r="E150" t="s">
-        <v>42</v>
+      <c r="E150">
+        <v>2</v>
       </c>
       <c r="F150" t="s">
         <v>25</v>
@@ -64606,8 +64683,8 @@
       <c r="D153" t="s">
         <v>23</v>
       </c>
-      <c r="E153" t="s">
-        <v>42</v>
+      <c r="E153">
+        <v>2</v>
       </c>
       <c r="F153" t="s">
         <v>25</v>
@@ -64774,8 +64851,8 @@
       <c r="D156" t="s">
         <v>23</v>
       </c>
-      <c r="E156" t="s">
-        <v>42</v>
+      <c r="E156">
+        <v>2</v>
       </c>
       <c r="F156" t="s">
         <v>25</v>
@@ -64942,8 +65019,8 @@
       <c r="D159" t="s">
         <v>23</v>
       </c>
-      <c r="E159" t="s">
-        <v>42</v>
+      <c r="E159">
+        <v>2</v>
       </c>
       <c r="F159" t="s">
         <v>25</v>
@@ -65110,8 +65187,8 @@
       <c r="D162" t="s">
         <v>23</v>
       </c>
-      <c r="E162" t="s">
-        <v>42</v>
+      <c r="E162">
+        <v>2</v>
       </c>
       <c r="F162" t="s">
         <v>25</v>
@@ -65278,8 +65355,8 @@
       <c r="D165" t="s">
         <v>23</v>
       </c>
-      <c r="E165" t="s">
-        <v>42</v>
+      <c r="E165">
+        <v>2</v>
       </c>
       <c r="F165" t="s">
         <v>25</v>
@@ -65446,8 +65523,8 @@
       <c r="D168" t="s">
         <v>23</v>
       </c>
-      <c r="E168" t="s">
-        <v>42</v>
+      <c r="E168">
+        <v>2</v>
       </c>
       <c r="F168" t="s">
         <v>25</v>
@@ -65614,8 +65691,8 @@
       <c r="D171" t="s">
         <v>23</v>
       </c>
-      <c r="E171" t="s">
-        <v>42</v>
+      <c r="E171">
+        <v>2</v>
       </c>
       <c r="F171" t="s">
         <v>25</v>
@@ -65782,8 +65859,8 @@
       <c r="D174" t="s">
         <v>23</v>
       </c>
-      <c r="E174" t="s">
-        <v>42</v>
+      <c r="E174">
+        <v>2</v>
       </c>
       <c r="F174" t="s">
         <v>25</v>
@@ -65950,8 +66027,8 @@
       <c r="D177" t="s">
         <v>23</v>
       </c>
-      <c r="E177" t="s">
-        <v>42</v>
+      <c r="E177">
+        <v>2</v>
       </c>
       <c r="F177" t="s">
         <v>25</v>
@@ -66118,8 +66195,8 @@
       <c r="D180" t="s">
         <v>23</v>
       </c>
-      <c r="E180" t="s">
-        <v>42</v>
+      <c r="E180">
+        <v>2</v>
       </c>
       <c r="F180" t="s">
         <v>25</v>
@@ -66286,8 +66363,8 @@
       <c r="D183" t="s">
         <v>23</v>
       </c>
-      <c r="E183" t="s">
-        <v>42</v>
+      <c r="E183">
+        <v>2</v>
       </c>
       <c r="F183" t="s">
         <v>25</v>
@@ -66454,8 +66531,8 @@
       <c r="D186" t="s">
         <v>23</v>
       </c>
-      <c r="E186" t="s">
-        <v>42</v>
+      <c r="E186">
+        <v>2</v>
       </c>
       <c r="F186" t="s">
         <v>25</v>
@@ -66622,8 +66699,8 @@
       <c r="D189" t="s">
         <v>23</v>
       </c>
-      <c r="E189" t="s">
-        <v>42</v>
+      <c r="E189">
+        <v>2</v>
       </c>
       <c r="F189" t="s">
         <v>25</v>
@@ -66790,8 +66867,8 @@
       <c r="D192" t="s">
         <v>23</v>
       </c>
-      <c r="E192" t="s">
-        <v>42</v>
+      <c r="E192">
+        <v>2</v>
       </c>
       <c r="F192" t="s">
         <v>25</v>
@@ -66958,8 +67035,8 @@
       <c r="D195" t="s">
         <v>23</v>
       </c>
-      <c r="E195" t="s">
-        <v>42</v>
+      <c r="E195">
+        <v>2</v>
       </c>
       <c r="F195" t="s">
         <v>25</v>
@@ -67126,8 +67203,8 @@
       <c r="D198" t="s">
         <v>23</v>
       </c>
-      <c r="E198" t="s">
-        <v>42</v>
+      <c r="E198">
+        <v>2</v>
       </c>
       <c r="F198" t="s">
         <v>25</v>
@@ -67294,8 +67371,8 @@
       <c r="D201" t="s">
         <v>23</v>
       </c>
-      <c r="E201" t="s">
-        <v>42</v>
+      <c r="E201">
+        <v>2</v>
       </c>
       <c r="F201" t="s">
         <v>25</v>
@@ -67462,8 +67539,8 @@
       <c r="D204" t="s">
         <v>23</v>
       </c>
-      <c r="E204" t="s">
-        <v>42</v>
+      <c r="E204">
+        <v>2</v>
       </c>
       <c r="F204" t="s">
         <v>25</v>
@@ -67630,8 +67707,8 @@
       <c r="D207" t="s">
         <v>23</v>
       </c>
-      <c r="E207" t="s">
-        <v>42</v>
+      <c r="E207">
+        <v>2</v>
       </c>
       <c r="F207" t="s">
         <v>25</v>
@@ -67798,8 +67875,8 @@
       <c r="D210" t="s">
         <v>23</v>
       </c>
-      <c r="E210" t="s">
-        <v>42</v>
+      <c r="E210">
+        <v>2</v>
       </c>
       <c r="F210" t="s">
         <v>25</v>
@@ -67842,6 +67919,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E210" xr:uid="{189C8868-C8D6-40DB-BD7E-3F95F87A70E9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>